<commit_message>
Thống kê báo cáo
</commit_message>
<xml_diff>
--- a/DocumentManage/DocumentManage/bin/Debug/Template/ThongKeCongTyDoVe.xlsx
+++ b/DocumentManage/DocumentManage/bin/Debug/Template/ThongKeCongTyDoVe.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>STT</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Phí thẩm định</t>
+  </si>
+  <si>
+    <t>Phường/xã</t>
   </si>
 </sst>
 </file>
@@ -83,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -93,6 +96,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -395,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -409,45 +415,47 @@
     <col min="5" max="6" width="17.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -457,7 +465,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -467,7 +475,20 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>